<commit_message>
Change lessor updated with the run manager
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager_Automatic_Renewal.xlsx
+++ b/src/test/resources/Run_Manager_Automatic_Renewal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\EjarUAT\EJAR_UAT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9572CCF0-F664-40F6-8027-B40EAA558E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C359A322-6E8A-4355-91D1-4F52F99CA486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="697" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="487">
   <si>
     <t>P_Key</t>
   </si>
@@ -1318,160 +1318,193 @@
     <t>ApproveAwqafResidentialSubleaseByTenantMoreThan3Months</t>
   </si>
   <si>
-    <t>WEB_TC_01</t>
-  </si>
-  <si>
-    <t>WEB_TC_02</t>
-  </si>
-  <si>
-    <t>WEB_TC_03</t>
-  </si>
-  <si>
-    <t>WEB_TC_04</t>
-  </si>
-  <si>
-    <t>WEB_TC_05</t>
-  </si>
-  <si>
-    <t>WEB_TC_06</t>
-  </si>
-  <si>
-    <t>WEB_TC_07</t>
-  </si>
-  <si>
-    <t>WEB_TC_08</t>
-  </si>
-  <si>
-    <t>WEB_TC_09</t>
-  </si>
-  <si>
-    <t>WEB_TC_10</t>
-  </si>
-  <si>
-    <t>WEB_TC_11</t>
-  </si>
-  <si>
-    <t>WEB_TC_12</t>
-  </si>
-  <si>
-    <t>WEB_TC_13</t>
-  </si>
-  <si>
-    <t>WEB_TC_14</t>
-  </si>
-  <si>
-    <t>WEB_TC_15</t>
-  </si>
-  <si>
-    <t>WEB_TC_16</t>
-  </si>
-  <si>
-    <t>WEB_TC_17</t>
-  </si>
-  <si>
-    <t>WEB_TC_18</t>
-  </si>
-  <si>
-    <t>WEB_TC_19</t>
-  </si>
-  <si>
-    <t>WEB_TC_20</t>
-  </si>
-  <si>
-    <t>WEB_TC_21</t>
-  </si>
-  <si>
-    <t>WEB_TC_22</t>
-  </si>
-  <si>
-    <t>WEB_TC_23</t>
-  </si>
-  <si>
-    <t>WEB_TC_24</t>
-  </si>
-  <si>
-    <t>WEB_TC_25</t>
-  </si>
-  <si>
-    <t>WEB_TC_26</t>
-  </si>
-  <si>
-    <t>WEB_TC_27</t>
-  </si>
-  <si>
-    <t>WEB_TC_28</t>
-  </si>
-  <si>
-    <t>WEB_TC_29</t>
-  </si>
-  <si>
-    <t>WEB_TC_30</t>
-  </si>
-  <si>
-    <t>WEB_TC_31</t>
-  </si>
-  <si>
-    <t>WEB_TC_32</t>
-  </si>
-  <si>
-    <t>WEB_TC_33</t>
-  </si>
-  <si>
-    <t>WEB_TC_34</t>
-  </si>
-  <si>
-    <t>WEB_TC_35</t>
-  </si>
-  <si>
-    <t>WEB_TC_36</t>
-  </si>
-  <si>
-    <t>WEB_TC_37</t>
-  </si>
-  <si>
-    <t>WEB_TC_38</t>
-  </si>
-  <si>
-    <t>WEB_TC_39</t>
-  </si>
-  <si>
     <t>AwqafResidentialSubleaseContractLessThan3Months</t>
   </si>
   <si>
-    <t>WEB_TC_40</t>
-  </si>
-  <si>
     <t>ApproveAwqafResidentialSubleaseByLesserLessThan3Months</t>
   </si>
   <si>
-    <t>WEB_TC_41</t>
-  </si>
-  <si>
     <t>ApproveAwqafResidentialSubleaseByTenantLessThan3Months</t>
   </si>
   <si>
-    <t>WEB_TC_42</t>
-  </si>
-  <si>
-    <t>WEB_TC_43</t>
-  </si>
-  <si>
-    <t>WEB_TC_44</t>
-  </si>
-  <si>
-    <t>WEB_TC_45</t>
-  </si>
-  <si>
-    <t>WEB_TC_46</t>
-  </si>
-  <si>
-    <t>WEB_TC_47</t>
-  </si>
-  <si>
-    <t>WEB_TC_48</t>
-  </si>
-  <si>
     <t>Precondition</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_01</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_02</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_03</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_04</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_05</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_06</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_07</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_08</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_09</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_10</t>
+  </si>
+  <si>
+    <t>AutomaticRenewal_TC_11</t>
+  </si>
+  <si>
+    <t>Contracts_TC_01</t>
+  </si>
+  <si>
+    <t>Contracts_TC_02</t>
+  </si>
+  <si>
+    <t>Contracts_TC_03</t>
+  </si>
+  <si>
+    <t>Contracts_TC_04</t>
+  </si>
+  <si>
+    <t>Contracts_TC_05</t>
+  </si>
+  <si>
+    <t>Contracts_TC_06</t>
+  </si>
+  <si>
+    <t>Contracts_TC_07</t>
+  </si>
+  <si>
+    <t>Contracts_TC_08</t>
+  </si>
+  <si>
+    <t>Contracts_TC_09</t>
+  </si>
+  <si>
+    <t>Contracts_TC_10</t>
+  </si>
+  <si>
+    <t>Contracts_TC_11</t>
+  </si>
+  <si>
+    <t>Contracts_TC_12</t>
+  </si>
+  <si>
+    <t>Contracts_TC_13</t>
+  </si>
+  <si>
+    <t>Contracts_TC_14</t>
+  </si>
+  <si>
+    <t>Contracts_TC_15</t>
+  </si>
+  <si>
+    <t>Contracts_TC_16</t>
+  </si>
+  <si>
+    <t>Contracts_TC_17</t>
+  </si>
+  <si>
+    <t>Contracts_TC_18</t>
+  </si>
+  <si>
+    <t>Contracts_TC_19</t>
+  </si>
+  <si>
+    <t>Contracts_TC_20</t>
+  </si>
+  <si>
+    <t>Contracts_TC_21</t>
+  </si>
+  <si>
+    <t>Contracts_TC_22</t>
+  </si>
+  <si>
+    <t>Contracts_TC_23</t>
+  </si>
+  <si>
+    <t>Contracts_TC_24</t>
+  </si>
+  <si>
+    <t>Contracts_TC_25</t>
+  </si>
+  <si>
+    <t>Contracts_TC_26</t>
+  </si>
+  <si>
+    <t>Contracts_TC_27</t>
+  </si>
+  <si>
+    <t>Contracts_TC_28</t>
+  </si>
+  <si>
+    <t>Contracts_TC_29</t>
+  </si>
+  <si>
+    <t>Contracts_TC_30</t>
+  </si>
+  <si>
+    <t>Contracts_TC_31</t>
+  </si>
+  <si>
+    <t>Contracts_TC_32</t>
+  </si>
+  <si>
+    <t>Contracts_TC_33</t>
+  </si>
+  <si>
+    <t>Contracts_TC_34</t>
+  </si>
+  <si>
+    <t>Contracts_TC_35</t>
+  </si>
+  <si>
+    <t>Contracts_TC_36</t>
+  </si>
+  <si>
+    <t>Contracts_TC_37</t>
+  </si>
+  <si>
+    <t>Contracts_TC_38</t>
+  </si>
+  <si>
+    <t>Contracts_TC_39</t>
+  </si>
+  <si>
+    <t>Contracts_TC_40</t>
+  </si>
+  <si>
+    <t>Contracts_TC_41</t>
+  </si>
+  <si>
+    <t>Contracts_TC_42</t>
+  </si>
+  <si>
+    <t>Contracts_TC_43</t>
+  </si>
+  <si>
+    <t>Contracts_TC_44</t>
+  </si>
+  <si>
+    <t>Contracts_TC_45</t>
+  </si>
+  <si>
+    <t>Contracts_TC_46</t>
+  </si>
+  <si>
+    <t>Contracts_TC_47</t>
+  </si>
+  <si>
+    <t>Contracts_TC_48</t>
   </si>
 </sst>
 </file>
@@ -2401,7 +2434,7 @@
       <selection activeCell="G5" sqref="G5"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2412,7 +2445,7 @@
     <col min="4" max="4" width="73" style="2" customWidth="1"/>
     <col min="5" max="5" width="40.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="13.21875" style="3" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -2465,7 +2498,7 @@
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
-        <v>475</v>
+        <v>427</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>265</v>
@@ -2512,7 +2545,7 @@
         <v>267</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>424</v>
+        <v>439</v>
       </c>
       <c r="H3" s="38" t="s">
         <v>246</v>
@@ -2521,7 +2554,7 @@
         <v>15</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K3" s="38">
         <v>1</v>
@@ -2551,7 +2584,7 @@
         <v>294</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="H4" s="38" t="s">
         <v>246</v>
@@ -2560,7 +2593,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K4" s="38">
         <v>1</v>
@@ -2590,7 +2623,7 @@
         <v>295</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>426</v>
+        <v>441</v>
       </c>
       <c r="H5" s="38" t="s">
         <v>246</v>
@@ -2599,7 +2632,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K5" s="38">
         <v>1</v>
@@ -2629,7 +2662,7 @@
         <v>267</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>427</v>
+        <v>442</v>
       </c>
       <c r="H6" s="38" t="s">
         <v>246</v>
@@ -2668,7 +2701,7 @@
         <v>294</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>428</v>
+        <v>443</v>
       </c>
       <c r="H7" s="38" t="s">
         <v>246</v>
@@ -2707,7 +2740,7 @@
         <v>295</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="H8" s="38" t="s">
         <v>246</v>
@@ -2746,7 +2779,7 @@
         <v>310</v>
       </c>
       <c r="G9" s="41" t="s">
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="H9" s="38" t="s">
         <v>246</v>
@@ -2785,7 +2818,7 @@
         <v>313</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>431</v>
+        <v>446</v>
       </c>
       <c r="H10" s="38" t="s">
         <v>246</v>
@@ -2824,7 +2857,7 @@
         <v>316</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="H11" s="38" t="s">
         <v>246</v>
@@ -2863,7 +2896,7 @@
         <v>310</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>433</v>
+        <v>448</v>
       </c>
       <c r="H12" s="38" t="s">
         <v>246</v>
@@ -2902,7 +2935,7 @@
         <v>313</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>434</v>
+        <v>449</v>
       </c>
       <c r="H13" s="38" t="s">
         <v>246</v>
@@ -2941,7 +2974,7 @@
         <v>316</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="H14" s="38" t="s">
         <v>246</v>
@@ -2980,7 +3013,7 @@
         <v>323</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>436</v>
+        <v>451</v>
       </c>
       <c r="H15" s="38" t="s">
         <v>246</v>
@@ -3019,7 +3052,7 @@
         <v>326</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>437</v>
+        <v>452</v>
       </c>
       <c r="H16" s="38" t="s">
         <v>246</v>
@@ -3058,7 +3091,7 @@
         <v>329</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>438</v>
+        <v>453</v>
       </c>
       <c r="H17" s="38" t="s">
         <v>246</v>
@@ -3097,7 +3130,7 @@
         <v>323</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>439</v>
+        <v>454</v>
       </c>
       <c r="H18" s="38" t="s">
         <v>246</v>
@@ -3136,7 +3169,7 @@
         <v>326</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>440</v>
+        <v>455</v>
       </c>
       <c r="H19" s="38" t="s">
         <v>246</v>
@@ -3175,7 +3208,7 @@
         <v>329</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="H20" s="38" t="s">
         <v>246</v>
@@ -3214,7 +3247,7 @@
         <v>323</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>442</v>
+        <v>457</v>
       </c>
       <c r="H21" s="38" t="s">
         <v>246</v>
@@ -3253,7 +3286,7 @@
         <v>326</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>443</v>
+        <v>458</v>
       </c>
       <c r="H22" s="38" t="s">
         <v>246</v>
@@ -3292,7 +3325,7 @@
         <v>329</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>444</v>
+        <v>459</v>
       </c>
       <c r="H23" s="38" t="s">
         <v>246</v>
@@ -3331,7 +3364,7 @@
         <v>323</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="H24" s="38" t="s">
         <v>246</v>
@@ -3370,7 +3403,7 @@
         <v>326</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>446</v>
+        <v>461</v>
       </c>
       <c r="H25" s="38" t="s">
         <v>246</v>
@@ -3409,7 +3442,7 @@
         <v>329</v>
       </c>
       <c r="G26" s="41" t="s">
-        <v>447</v>
+        <v>462</v>
       </c>
       <c r="H26" s="38" t="s">
         <v>246</v>
@@ -3448,7 +3481,7 @@
         <v>346</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>448</v>
+        <v>463</v>
       </c>
       <c r="H27" s="38" t="s">
         <v>246</v>
@@ -3487,7 +3520,7 @@
         <v>349</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>449</v>
+        <v>464</v>
       </c>
       <c r="H28" s="38" t="s">
         <v>246</v>
@@ -3526,7 +3559,7 @@
         <v>352</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>450</v>
+        <v>465</v>
       </c>
       <c r="H29" s="38" t="s">
         <v>246</v>
@@ -3565,7 +3598,7 @@
         <v>346</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>451</v>
+        <v>466</v>
       </c>
       <c r="H30" s="38" t="s">
         <v>246</v>
@@ -3604,7 +3637,7 @@
         <v>349</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>452</v>
+        <v>467</v>
       </c>
       <c r="H31" s="38" t="s">
         <v>246</v>
@@ -3643,7 +3676,7 @@
         <v>352</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>453</v>
+        <v>468</v>
       </c>
       <c r="H32" s="38" t="s">
         <v>246</v>
@@ -3682,7 +3715,7 @@
         <v>346</v>
       </c>
       <c r="G33" s="41" t="s">
-        <v>454</v>
+        <v>469</v>
       </c>
       <c r="H33" s="38" t="s">
         <v>246</v>
@@ -3721,7 +3754,7 @@
         <v>349</v>
       </c>
       <c r="G34" s="41" t="s">
-        <v>455</v>
+        <v>470</v>
       </c>
       <c r="H34" s="38" t="s">
         <v>246</v>
@@ -3760,7 +3793,7 @@
         <v>352</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>456</v>
+        <v>471</v>
       </c>
       <c r="H35" s="38" t="s">
         <v>246</v>
@@ -3799,7 +3832,7 @@
         <v>346</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>457</v>
+        <v>472</v>
       </c>
       <c r="H36" s="38" t="s">
         <v>246</v>
@@ -3838,7 +3871,7 @@
         <v>349</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>458</v>
+        <v>473</v>
       </c>
       <c r="H37" s="38" t="s">
         <v>246</v>
@@ -3877,7 +3910,7 @@
         <v>352</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>459</v>
+        <v>474</v>
       </c>
       <c r="H38" s="38" t="s">
         <v>246</v>
@@ -3916,7 +3949,7 @@
         <v>373</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>460</v>
+        <v>475</v>
       </c>
       <c r="H39" s="38" t="s">
         <v>246</v>
@@ -3955,7 +3988,7 @@
         <v>376</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>461</v>
+        <v>476</v>
       </c>
       <c r="H40" s="38" t="s">
         <v>246</v>
@@ -3994,7 +4027,7 @@
         <v>379</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>462</v>
+        <v>477</v>
       </c>
       <c r="H41" s="38" t="s">
         <v>246</v>
@@ -4027,13 +4060,13 @@
         <v>288</v>
       </c>
       <c r="E42" s="41" t="s">
-        <v>463</v>
+        <v>424</v>
       </c>
       <c r="F42" s="41" t="s">
         <v>373</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="H42" s="38" t="s">
         <v>246</v>
@@ -4066,13 +4099,13 @@
         <v>370</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="F43" s="41" t="s">
         <v>376</v>
       </c>
       <c r="G43" s="41" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="H43" s="38" t="s">
         <v>246</v>
@@ -4105,13 +4138,13 @@
         <v>371</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>467</v>
+        <v>426</v>
       </c>
       <c r="F44" s="41" t="s">
         <v>379</v>
       </c>
       <c r="G44" s="41" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="H44" s="38" t="s">
         <v>246</v>
@@ -4150,7 +4183,7 @@
         <v>373</v>
       </c>
       <c r="G45" s="41" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="H45" s="38" t="s">
         <v>246</v>
@@ -4189,7 +4222,7 @@
         <v>376</v>
       </c>
       <c r="G46" s="41" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="H46" s="38" t="s">
         <v>246</v>
@@ -4228,7 +4261,7 @@
         <v>379</v>
       </c>
       <c r="G47" s="41" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="H47" s="38" t="s">
         <v>246</v>
@@ -4267,7 +4300,7 @@
         <v>373</v>
       </c>
       <c r="G48" s="41" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="H48" s="38" t="s">
         <v>246</v>
@@ -4306,7 +4339,7 @@
         <v>376</v>
       </c>
       <c r="G49" s="41" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="H49" s="38" t="s">
         <v>246</v>
@@ -4345,7 +4378,7 @@
         <v>379</v>
       </c>
       <c r="G50" s="41" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="H50" s="38" t="s">
         <v>246</v>
@@ -4410,8 +4443,8 @@
       <c r="F52" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="G52" s="48" t="s">
-        <v>383</v>
+      <c r="G52" s="41" t="s">
+        <v>428</v>
       </c>
       <c r="H52" s="38" t="s">
         <v>246</v>
@@ -4449,8 +4482,8 @@
       <c r="F53" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="G53" s="48" t="s">
-        <v>386</v>
+      <c r="G53" s="41" t="s">
+        <v>429</v>
       </c>
       <c r="H53" s="38" t="s">
         <v>246</v>
@@ -4488,8 +4521,8 @@
       <c r="F54" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="G54" s="48" t="s">
-        <v>388</v>
+      <c r="G54" s="41" t="s">
+        <v>430</v>
       </c>
       <c r="H54" s="38" t="s">
         <v>246</v>
@@ -4528,7 +4561,7 @@
         <v>385</v>
       </c>
       <c r="G55" s="41" t="s">
-        <v>264</v>
+        <v>431</v>
       </c>
       <c r="H55" s="38" t="s">
         <v>246</v>
@@ -4566,7 +4599,7 @@
         <v>393</v>
       </c>
       <c r="G56" s="41" t="s">
-        <v>391</v>
+        <v>432</v>
       </c>
       <c r="H56" s="38" t="s">
         <v>246</v>
@@ -4604,7 +4637,7 @@
         <v>385</v>
       </c>
       <c r="G57" s="41" t="s">
-        <v>394</v>
+        <v>433</v>
       </c>
       <c r="H57" s="38" t="s">
         <v>246</v>
@@ -4642,7 +4675,7 @@
         <v>398</v>
       </c>
       <c r="G58" s="41" t="s">
-        <v>396</v>
+        <v>434</v>
       </c>
       <c r="H58" s="38" t="s">
         <v>246</v>
@@ -4680,7 +4713,7 @@
         <v>398</v>
       </c>
       <c r="G59" s="41" t="s">
-        <v>399</v>
+        <v>435</v>
       </c>
       <c r="H59" s="38" t="s">
         <v>246</v>
@@ -4718,7 +4751,7 @@
         <v>398</v>
       </c>
       <c r="G60" s="41" t="s">
-        <v>401</v>
+        <v>436</v>
       </c>
       <c r="H60" s="38" t="s">
         <v>246</v>
@@ -4756,7 +4789,7 @@
         <v>398</v>
       </c>
       <c r="G61" s="41" t="s">
-        <v>403</v>
+        <v>437</v>
       </c>
       <c r="H61" s="38" t="s">
         <v>246</v>
@@ -4794,7 +4827,7 @@
         <v>398</v>
       </c>
       <c r="G62" s="41" t="s">
-        <v>405</v>
+        <v>438</v>
       </c>
       <c r="H62" s="38" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
Batch runner is added
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager_Automatic_Renewal.xlsx
+++ b/src/test/resources/Run_Manager_Automatic_Renewal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\EjarUAT\EJAR_UAT\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\EjarUAT\EJAR_STG_R1-main\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C359A322-6E8A-4355-91D1-4F52F99CA486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD05CB1C-C8C0-4C37-B424-DC9C0FCCCBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="697" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="488">
   <si>
     <t>P_Key</t>
   </si>
@@ -1505,6 +1505,9 @@
   </si>
   <si>
     <t>Contracts_TC_48</t>
+  </si>
+  <si>
+    <t>Regression</t>
   </si>
 </sst>
 </file>
@@ -2434,7 +2437,7 @@
       <selection activeCell="G5" sqref="G5"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2554,7 +2557,7 @@
         <v>15</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="K3" s="38">
         <v>1</v>
@@ -2593,7 +2596,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="K4" s="38">
         <v>1</v>
@@ -2632,7 +2635,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="K5" s="38">
         <v>1</v>
@@ -4450,7 +4453,7 @@
         <v>246</v>
       </c>
       <c r="I52" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J52" s="42" t="s">
         <v>28</v>
@@ -4489,7 +4492,7 @@
         <v>246</v>
       </c>
       <c r="I53" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J53" s="42" t="s">
         <v>28</v>
@@ -4528,7 +4531,7 @@
         <v>246</v>
       </c>
       <c r="I54" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J54" s="42" t="s">
         <v>28</v>
@@ -4567,7 +4570,7 @@
         <v>246</v>
       </c>
       <c r="I55" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J55" s="42" t="s">
         <v>28</v>
@@ -4605,7 +4608,7 @@
         <v>246</v>
       </c>
       <c r="I56" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J56" s="42" t="s">
         <v>28</v>
@@ -4643,7 +4646,7 @@
         <v>246</v>
       </c>
       <c r="I57" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J57" s="42" t="s">
         <v>28</v>
@@ -4681,7 +4684,7 @@
         <v>246</v>
       </c>
       <c r="I58" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J58" s="42" t="s">
         <v>28</v>
@@ -4719,7 +4722,7 @@
         <v>246</v>
       </c>
       <c r="I59" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J59" s="42" t="s">
         <v>28</v>
@@ -4757,7 +4760,7 @@
         <v>246</v>
       </c>
       <c r="I60" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J60" s="42" t="s">
         <v>28</v>
@@ -4795,7 +4798,7 @@
         <v>246</v>
       </c>
       <c r="I61" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J61" s="42" t="s">
         <v>28</v>
@@ -4833,7 +4836,7 @@
         <v>246</v>
       </c>
       <c r="I62" s="38" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
       <c r="J62" s="42" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Nafath Login is implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager_Automatic_Renewal.xlsx
+++ b/src/test/resources/Run_Manager_Automatic_Renewal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\EjarUAT\EJAR_STG_R1-main\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD05CB1C-C8C0-4C37-B424-DC9C0FCCCBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A914475-2BF6-4C25-A3D7-C8E2BA5E26D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="697" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2437,7 +2437,7 @@
       <selection activeCell="G5" sqref="G5"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2635,7 +2635,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K5" s="38">
         <v>1</v>
@@ -7738,7 +7738,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7867,7 +7867,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>